<commit_message>
Added more code and documentation
</commit_message>
<xml_diff>
--- a/COMP 5280 - Introduction to Artificial Intelligence/COMP5280 - Introduction to Artificial Intelligence Cheatsheet.xlsx
+++ b/COMP 5280 - Introduction to Artificial Intelligence/COMP5280 - Introduction to Artificial Intelligence Cheatsheet.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livekentac-my.sharepoint.com/personal/cw734_kent_ac_uk/Documents/Year 2/Year 2 Coursework and Exam Notes/Introduction to Artificial Intelligence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livekentac-my.sharepoint.com/personal/cw734_kent_ac_uk/Documents/Year 2/COMP 5280 - Introduction to Artificial Intelligence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{471A402C-CAF4-4F7F-BCC3-137E744B60A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4286340B-2C71-4879-85E6-FD3AB64AA946}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{471A402C-CAF4-4F7F-BCC3-137E744B60A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70B5B780-D645-4802-8A4D-798FC35EF212}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" activeTab="1" xr2:uid="{88828811-411B-437D-A465-BC25B6ED090C}"/>
+    <workbookView xWindow="7680" yWindow="204" windowWidth="23040" windowHeight="12120" activeTab="3" xr2:uid="{88828811-411B-437D-A465-BC25B6ED090C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lecture 1 - Introduction" sheetId="1" r:id="rId1"/>
-    <sheet name="Lecture 2 - Serach (1)" sheetId="2" r:id="rId2"/>
+    <sheet name="L1 - Introduction" sheetId="1" r:id="rId1"/>
+    <sheet name="L2 - Search (1)" sheetId="2" r:id="rId2"/>
+    <sheet name="L3 - Search (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="L4 - Breadth+Depth First Search" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,11 +39,11 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="15">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -56,20 +58,150 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="15">
     <bk>
       <rc t="1" v="0"/>
     </bk>
     <bk>
       <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Concept</t>
   </si>
@@ -256,6 +388,126 @@
     <t>- If the state space is small, you can find a solution quickly (e.g. brute force, simple manual counting)
 - If the state space is large, you may need to use a path-finding algorithm, as brute force may not work</t>
   </si>
+  <si>
+    <t>Recalling the Search Problem</t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>For our purpose, a graph is a structure where nodes (also vertices) are connected by edges</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> graph G is a pair (V, E), where
+- V is a set of vertices
+- E ⊆ V × V is a set of edges (between the vertices)
+Graphs can be directed (edges have an orientation) or undirected.</t>
+  </si>
+  <si>
+    <t>State Space Graph</t>
+  </si>
+  <si>
+    <t>A mathematical representatino  of a search problem,  as abstracted into directed graphs</t>
+  </si>
+  <si>
+    <t>Facts about state space graphs:
+- Nodes are (abstracted) states
+- Edges are actions (connect states to successors)
+- Some nodes are goal nodes
+- A solution is a path in the graph
+State space graphs are finite, because every state only occurs once.</t>
+  </si>
+  <si>
+    <t>Search Tree</t>
+  </si>
+  <si>
+    <t>A tree of all possible action sequences from the start state. Essentially it's another type of abstraction to show all possible explorations</t>
+  </si>
+  <si>
+    <t>Facts about search trees:
+- The root node is the start state
+- Children correspond to successors
+- Nodes correspond to paths to achieve states they are referencing
+There is a lot of repeated structure with this format</t>
+  </si>
+  <si>
+    <t>Pacman example using state space graph</t>
+  </si>
+  <si>
+    <t>Pacman example using search tree</t>
+  </si>
+  <si>
+    <t>Generic Tree Search Algorithm</t>
+  </si>
+  <si>
+    <t>Methodically explore the search space (the search tree) by trying all possible paths</t>
+  </si>
+  <si>
+    <t>Steps associated with generic tree search algorithm:
+- Incrementally explore paths from the start node
+- Maintain a frontier of paths that have been explored
+- Expand the frontier to uncover unexplored paths
+One of the key features that is relevant for a generic tree search algorithm is that the order in which nodes from the frontier are expanded defines the search/exploration strategy.
+Search algorithms must also attempt to implement recursive behaviour in a loop, as we don't know how long it will take to find the correct path/won't find the path</t>
+  </si>
+  <si>
+    <t>Search Algorithm Properties</t>
+  </si>
+  <si>
+    <t>Completeness - does it always find a solution if one exists?
+Optimality - does it always find a least-cost solution?
+Time complexity - number of nodes generated/ expanded
+Space complexity - maximum number of nodes in memory</t>
+  </si>
+  <si>
+    <t>Depth-First Search</t>
+  </si>
+  <si>
+    <t>Depth-First Search means that it will only search a single pathway at a time - it will get to the end of a pathway. If it reaches the end of a pathway, it will go back up as few layers as possible to find the next branching path.</t>
+  </si>
+  <si>
+    <t>Breadth-First Search</t>
+  </si>
+  <si>
+    <t>Breadth-First Search refers to when the search is done by prioritising the breadth of each individual node before the depth.</t>
+  </si>
+  <si>
+    <t>Depth-First  Search refers to when the search is done by prioritising the depth of each individual node before the breadth.</t>
+  </si>
+  <si>
+    <t>Breadh-First Search will allow for multiple pathways to be transferred at the same time. However the pathway will be explored at a slower rate (at a reduced depth).</t>
+  </si>
+  <si>
+    <t>Cost-Sensitive Searches</t>
+  </si>
+  <si>
+    <t>Cost-sensitive searches refer to search strategies that take into account the varying costs associated with different search actions or outcomes.</t>
+  </si>
+  <si>
+    <t>In cost-sensitive searches, the traditional notion of simply maximizing the number of successful outcomes is re-evaluated by incorporating the costs associated with various search paths. This approach acknowledges that not all decisions yield equal benefits; some may incur higher risks or expenses. For instance, in an information retrieval scenario, the cost of processing irrelevant data might outweigh the benefit of retrieving useful information. By factoring in these varying costs, algorithms can be optimized to not only enhance efficiency but also improve overall outcomes, leading to more informed and strategic decision-making. This method finds applications in various fields, from computer science and economics to healthcare, where resource allocation and risk management are critical.</t>
+  </si>
+  <si>
+    <t>Uniform Cost (Least-Cost First) Search</t>
+  </si>
+  <si>
+    <t>Uniform Cost Search is a search algorithm that determines the path it's going to take based on the cumulative cost of travelling along the path, ensuring that the least expensive option is always expanded first.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N/A - All notes included within </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L3 - Search (2)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -343,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -360,14 +612,42 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+  <dxfs count="19">
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -413,16 +693,20 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -449,6 +733,14 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -458,11 +750,29 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -475,6 +785,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,7 +832,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="15">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -527,6 +841,58 @@
     <v>1</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -543,11 +909,24 @@
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
   <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
 </richValueRels>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D81F8203-8AEC-44BA-9534-F2EEBD7F49BB}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D81F8203-8AEC-44BA-9534-F2EEBD7F49BB}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:D2" xr:uid="{D81F8203-8AEC-44BA-9534-F2EEBD7F49BB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{16B75F82-3508-49D9-B98B-068A0F957CD4}" name="Concept"/>
@@ -560,13 +939,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{72EE0A3A-BF4B-4317-97BE-4D57194981F7}" name="Table13" displayName="Table13" ref="A1:D7" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
-  <autoFilter ref="A1:D7" xr:uid="{72EE0A3A-BF4B-4317-97BE-4D57194981F7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{72EE0A3A-BF4B-4317-97BE-4D57194981F7}" name="Table13" displayName="Table13" ref="A1:D8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="A1:D8" xr:uid="{72EE0A3A-BF4B-4317-97BE-4D57194981F7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3CB3DB59-5D29-401B-8E57-B4D22EA9BE1D}" name="Concept" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B9BCB745-5BE5-45C2-8C34-85EC476C7703}" name="Simple Explanation" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{484FEFBB-5D52-4A05-AD8D-E5DFE592E730}" name="More Details" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{397B2E5B-D4BF-4911-8144-EC1A6DEC4319}" name="Images" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3CB3DB59-5D29-401B-8E57-B4D22EA9BE1D}" name="Concept" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{B9BCB745-5BE5-45C2-8C34-85EC476C7703}" name="Simple Explanation" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{484FEFBB-5D52-4A05-AD8D-E5DFE592E730}" name="More Details" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{397B2E5B-D4BF-4911-8144-EC1A6DEC4319}" name="Images" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6688487E-9F1D-4C2F-AFA1-ABC938B771C3}" name="Table3" displayName="Table3" ref="A1:D12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="A1:D12" xr:uid="{6688487E-9F1D-4C2F-AFA1-ABC938B771C3}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8EF8BB02-070E-483F-9E56-02D3E16E9BDB}" name="Concept" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{794466AF-F6CF-4339-8E51-FE3B2E8E8E4A}" name="Simple Explanation" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{938F5D8A-8701-4E1B-890B-6B0E2F852EED}" name="More Details" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{57D5DFB1-914E-46B8-AA9A-8A8C2D3A12BB}" name="Images" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -887,6 +1279,26 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="2">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8F1D64F6-9B35-4998-ADAA-1102F9F8A4BB}">
+  <we:reference id="wa200005669" version="2.0.0.0" store="en-GB" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200005669" version="2.0.0.0" store="wa200005669" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D701999-4B13-40B4-A325-8C3869DA5B26}">
   <dimension ref="A1:D2"/>
@@ -930,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C4A009-66D7-4140-BD70-436559DEF170}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,6 +1425,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="210" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1022,6 +1442,205 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03143B44-1E82-42D3-B3D0-8C86B8761F3C}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="64.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="82.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="73.88671875" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="8" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="8" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="8" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="231.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="8" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="155.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="180" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="8" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="232.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="204.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="8" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E9" s="8" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="219.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="8" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E10" s="8" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="216" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="8" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8648DF-499A-4B81-8B1A-E79EFE4F7518}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{51a9fa56-3f32-449a-a721-3e3f49aa5e9a}" enabled="0" method="" siteId="{51a9fa56-3f32-449a-a721-3e3f49aa5e9a}" removed="1"/>

</xml_diff>